<commit_message>
add growth chart in the front page
</commit_message>
<xml_diff>
--- a/analytics/Informed_Investing_Template.xlsx
+++ b/analytics/Informed_Investing_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/q479070/Documents/personal_workspace/informed_investing/analytics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB38A121-1CF3-9746-8D77-305D35EA0CD5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DAC9B69-B2CE-3A43-849F-904A11007405}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14640" yWindow="2660" windowWidth="18960" windowHeight="17440" xr2:uid="{30D80B9D-1700-C74A-B972-4D2EFBDEA322}"/>
+    <workbookView xWindow="940" yWindow="460" windowWidth="32660" windowHeight="20540" xr2:uid="{30D80B9D-1700-C74A-B972-4D2EFBDEA322}"/>
   </bookViews>
   <sheets>
     <sheet name="INPUT" sheetId="1" r:id="rId1"/>
@@ -28,20 +28,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="72">
-  <si>
-    <t>GOOGL</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="75">
   <si>
     <t>FINANCIAL YEAR</t>
   </si>
@@ -254,6 +246,18 @@
   </si>
   <si>
     <t>Equity Growth</t>
+  </si>
+  <si>
+    <t>Fair value calculation:</t>
+  </si>
+  <si>
+    <t>(B4*INPUT!B17*(1+E4)^B5)/(1+B8)^B5</t>
+  </si>
+  <si>
+    <t>(EPS * AVG PE * (GROWTH_EST ^ YR) ) / REQUIRED RETURN RATE ^ YR</t>
+  </si>
+  <si>
+    <t>amzn</t>
   </si>
 </sst>
 </file>
@@ -265,7 +269,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="35">
+  <fonts count="37">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -494,6 +498,20 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -693,10 +711,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="36" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -771,17 +790,10 @@
     <xf numFmtId="10" fontId="29" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="8" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -845,12 +857,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="32" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="32" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -872,16 +878,39 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="32" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="32" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFBA20B1"/>
       <color rgb="FF9D0AEC"/>
-      <color rgb="FFBA20B1"/>
     </mruColors>
   </colors>
   <extLst>
@@ -896,6 +925,1074 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>GROWTH</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'GROWTH YoY'!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SALES ($m.)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="60000"/>
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="60000"/>
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'GROWTH YoY'!$B$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2015</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'GROWTH YoY'!$B$3:$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-721B-7F4B-9F27-CE8577B028E3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'GROWTH YoY'!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EPS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'GROWTH YoY'!$B$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2015</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'GROWTH YoY'!$B$4:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-721B-7F4B-9F27-CE8577B028E3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'GROWTH YoY'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EQUITY ($m.)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'GROWTH YoY'!$B$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2015</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'GROWTH YoY'!$B$5:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-721B-7F4B-9F27-CE8577B028E3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'GROWTH YoY'!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FCF ($m.)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="BA20B1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent6">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent6">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'GROWTH YoY'!$B$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2015</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'GROWTH YoY'!$B$6:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-721B-7F4B-9F27-CE8577B028E3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'GROWTH YoY'!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ROIC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'GROWTH YoY'!$B$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2015</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'GROWTH YoY'!$B$7:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-721B-7F4B-9F27-CE8577B028E3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'GROWTH YoY'!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AVG GROWTH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg2"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="60000"/>
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="60000"/>
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'GROWTH YoY'!$B$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2015</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'GROWTH YoY'!$B$8:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-721B-7F4B-9F27-CE8577B028E3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="133143392"/>
+        <c:axId val="133145696"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="133143392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="133145696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="133145696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="-0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="133143392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.5"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="tr"/>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1039,16 +2136,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.23421586757475973</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.23110947474870097</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.22193925428985023</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.19991083246218541</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1127,16 +2224,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.427777777777778</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25264531582293448</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.24144775025901291</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.20729050855011433</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1213,16 +2310,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.16475849497055775</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.13029571332072334</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1386177942897116</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.14357796061274317</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1299,16 +2396,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>-4.4822127801382922E-2</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-6.2046099239995232E-2</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.11242077175800112</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.17413810344383429</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1389,16 +2486,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.1557734204793022</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.10186679296902529</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.5284737673440077E-2</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.5688936024080485E-2</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1617,7 +2714,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1762,16 +2859,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.23421586757475982</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.22801090038993266</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.20380322447292271</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.13617975485219921</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1851,16 +2948,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.427777777777778</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.35368043087971279</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.21935201401050794</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11035488575595526</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1887,7 +2984,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="31750" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -1938,16 +3035,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.16475849497055775</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.685261371155672E-2</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15544622748917569</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.15858848449836319</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2025,16 +3122,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>-4.4822127801382991E-2</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-7.8959484346224684E-2</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.56474755358107698</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.38060505594695399</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2116,16 +3213,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.1557734204793024</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.43680981595092017</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-4.276114844227262E-3</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-4.8255813953488276E-2</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2134,6 +3231,98 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-3A36-3F45-A679-8EAF9D262BFF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'GROWTH YoY'!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AVG GROWTH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'GROWTH YoY'!$B$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2015</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'GROWTH YoY'!$B$8:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D956-7640-9281-5313378697FF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2418,7 +3607,546 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2921,7 +4649,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3425,6 +5153,49 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>215900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>215900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFE3CBCC-B4F7-4F49-8BDA-D483AD3E061C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3467,7 +5238,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3828,7 +5599,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -3841,266 +5612,266 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="31">
+        <v>74</v>
+      </c>
+      <c r="C1" s="31" t="e">
         <f ca="1">[1]!QFS(INPUT!$B$1, "price")</f>
-        <v>1044.6400000000001</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="F3" s="13" t="s">
         <v>34</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="28">
+        <v>1</v>
+      </c>
+      <c r="B4" s="28" t="e">
         <f ca="1">[1]!QFS($B$1, "revenue", $B$3)</f>
-        <v>66001</v>
-      </c>
-      <c r="C4" s="28">
+        <v>#N/A</v>
+      </c>
+      <c r="C4" s="28" t="e">
         <f ca="1">[1]!QFS($B$1, "revenue", $C$3)</f>
-        <v>74989</v>
-      </c>
-      <c r="D4" s="28">
+        <v>#N/A</v>
+      </c>
+      <c r="D4" s="28" t="e">
         <f ca="1">[1]!QFS($B$1, "revenue", $D$3)</f>
-        <v>90272</v>
-      </c>
-      <c r="E4" s="28">
+        <v>#N/A</v>
+      </c>
+      <c r="E4" s="28" t="e">
         <f ca="1">[1]!QFS($B$1, "revenue", $E$3)</f>
-        <v>110855</v>
-      </c>
-      <c r="F4" s="28">
+        <v>#N/A</v>
+      </c>
+      <c r="F4" s="28" t="e">
         <f ca="1">[1]!QFS($B$1, "revenue", $F$3)</f>
-        <v>136819</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="28">
+        <v>2</v>
+      </c>
+      <c r="B5" s="28" t="e">
         <f ca="1">[1]!QFS($B$1, "eps_diluted", $B$3)</f>
-        <v>20.57</v>
-      </c>
-      <c r="C5" s="28">
+        <v>#N/A</v>
+      </c>
+      <c r="C5" s="28" t="e">
         <f ca="1">[1]!QFS($B$1, "eps_diluted", $C$3)</f>
-        <v>22.84</v>
-      </c>
-      <c r="D5" s="28">
+        <v>#N/A</v>
+      </c>
+      <c r="D5" s="28" t="e">
         <f ca="1">[1]!QFS($B$1, "eps_diluted", $D$3)</f>
-        <v>27.85</v>
-      </c>
-      <c r="E5" s="28">
+        <v>#N/A</v>
+      </c>
+      <c r="E5" s="28" t="e">
         <f ca="1">[1]!QFS($B$1, "eps_diluted", $E$3)</f>
-        <v>18</v>
-      </c>
-      <c r="F5" s="28">
+        <v>#N/A</v>
+      </c>
+      <c r="F5" s="28" t="e">
         <f ca="1">[1]!QFS($B$1, "eps_diluted", $F$3)</f>
-        <v>43.7</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="28">
+        <v>3</v>
+      </c>
+      <c r="B6" s="28" t="e">
         <f ca="1">[1]!QFS($B$1, "total_equity", $B$3)</f>
-        <v>103860</v>
-      </c>
-      <c r="C6" s="28">
+        <v>#N/A</v>
+      </c>
+      <c r="C6" s="28" t="e">
         <f ca="1">[1]!QFS($B$1, "total_equity", $C$3)</f>
-        <v>120331</v>
-      </c>
-      <c r="D6" s="28">
+        <v>#N/A</v>
+      </c>
+      <c r="D6" s="28" t="e">
         <f ca="1">[1]!QFS($B$1, "total_equity", $D$3)</f>
-        <v>139036</v>
-      </c>
-      <c r="E6" s="28">
+        <v>#N/A</v>
+      </c>
+      <c r="E6" s="28" t="e">
         <f ca="1">[1]!QFS($B$1, "total_equity", $E$3)</f>
-        <v>152502</v>
-      </c>
-      <c r="F6" s="28">
+        <v>#N/A</v>
+      </c>
+      <c r="F6" s="28" t="e">
         <f ca="1">[1]!QFS($B$1, "total_equity", $F$3)</f>
-        <v>177628</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="28">
+        <v>4</v>
+      </c>
+      <c r="B7" s="28" t="e">
         <f ca="1">[1]!QFS($B$1, "fcf", $B$3)</f>
-        <v>12065</v>
-      </c>
-      <c r="C7" s="28">
+        <v>#N/A</v>
+      </c>
+      <c r="C7" s="28" t="e">
         <f ca="1">[1]!QFS($B$1, "fcf", $C$3)</f>
-        <v>16657</v>
-      </c>
-      <c r="D7" s="28">
+        <v>#N/A</v>
+      </c>
+      <c r="D7" s="28" t="e">
         <f ca="1">[1]!QFS($B$1, "fcf", $D$3)</f>
-        <v>26064</v>
-      </c>
-      <c r="E7" s="28">
+        <v>#N/A</v>
+      </c>
+      <c r="E7" s="28" t="e">
         <f ca="1">[1]!QFS($B$1, "fcf", $E$3)</f>
-        <v>24006</v>
-      </c>
-      <c r="F7" s="28">
+        <v>#N/A</v>
+      </c>
+      <c r="F7" s="28" t="e">
         <f ca="1">[1]!QFS($B$1, "fcf", $F$3)</f>
-        <v>22930</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="29">
+        <v>29</v>
+      </c>
+      <c r="B8" s="29" t="e">
         <f ca="1">[1]!QFS($B$1, "roic", $B$3) * 100</f>
-        <v>17.2</v>
-      </c>
-      <c r="C8" s="29">
+        <v>#N/A</v>
+      </c>
+      <c r="C8" s="29" t="e">
         <f ca="1">[1]!QFS($B$1, "roic", $C$3) * 100</f>
-        <v>16.37</v>
-      </c>
-      <c r="D8" s="29">
+        <v>#N/A</v>
+      </c>
+      <c r="D8" s="29" t="e">
         <f ca="1">[1]!QFS($B$1, "roic", $D$3) * 100</f>
-        <v>16.3</v>
-      </c>
-      <c r="E8" s="29">
+        <v>#N/A</v>
+      </c>
+      <c r="E8" s="29" t="e">
         <f ca="1">[1]!QFS($B$1, "roic", $E$3) * 100</f>
-        <v>9.1800000000000015</v>
-      </c>
-      <c r="F8" s="29">
+        <v>#N/A</v>
+      </c>
+      <c r="F8" s="29" t="e">
         <f ca="1">[1]!QFS($B$1, "roic", $F$3) * 100</f>
-        <v>19.79</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
-      <c r="F9" s="28">
+      <c r="F9" s="28" t="e">
         <f ca="1">[1]!QFS($B$1, "total_current_assets", $F$3)</f>
-        <v>135676</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
-      <c r="F10" s="28">
+      <c r="F10" s="28" t="e">
         <f ca="1">[1]!QFS($B$1, "total_current_liabilities", $F$3)</f>
-        <v>34620</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
       <c r="D11" s="22"/>
       <c r="E11" s="22"/>
-      <c r="F11" s="28">
+      <c r="F11" s="28" t="e">
         <f ca="1">[1]!QFS($B$1, "total_liabilities", $F$3)</f>
-        <v>55164</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="34"/>
       <c r="C14" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="40" t="s">
+      <c r="E14" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="40" t="s">
+      <c r="F14" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="40" t="s">
+      <c r="G14" s="41" t="s">
         <v>34</v>
-      </c>
-      <c r="G14" s="41" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="35">
+        <v>11</v>
+      </c>
+      <c r="B15" s="35" t="e">
         <f ca="1">MIN(C15:G15)</f>
-        <v>23.647600000000001</v>
-      </c>
-      <c r="C15" s="36">
+        <v>#N/A</v>
+      </c>
+      <c r="C15" s="36" t="e">
         <f ca="1">[1]!QFS(INPUT!$B$1, "price_to_earnings", C14)</f>
-        <v>25.570499999999999</v>
-      </c>
-      <c r="D15" s="37">
+        <v>#N/A</v>
+      </c>
+      <c r="D15" s="37" t="e">
         <f ca="1">[1]!QFS(INPUT!$B$1, "price_to_earnings", D14)</f>
-        <v>32.711399999999998</v>
-      </c>
-      <c r="E15" s="37">
+        <v>#N/A</v>
+      </c>
+      <c r="E15" s="37" t="e">
         <f ca="1">[1]!QFS(INPUT!$B$1, "price_to_earnings", E14)</f>
-        <v>28.124700000000001</v>
-      </c>
-      <c r="F15" s="37">
+        <v>#N/A</v>
+      </c>
+      <c r="F15" s="37" t="e">
         <f ca="1">[1]!QFS(INPUT!$B$1, "price_to_earnings", F14)</f>
-        <v>57.801400000000001</v>
-      </c>
-      <c r="G15" s="38">
+        <v>#N/A</v>
+      </c>
+      <c r="G15" s="38" t="e">
         <f ca="1">[1]!QFS(INPUT!$B$1, "price_to_earnings", G14)</f>
-        <v>23.647600000000001</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="30">
+        <v>12</v>
+      </c>
+      <c r="B16" s="30" t="e">
         <f ca="1">MAX(C15:G15)</f>
-        <v>57.801400000000001</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="30">
+        <v>13</v>
+      </c>
+      <c r="B17" s="30" t="e">
         <f ca="1">AVERAGE(C15:G15)</f>
-        <v>33.571120000000001</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -4109,26 +5880,26 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19" s="14"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="30">
+        <v>15</v>
+      </c>
+      <c r="B20" s="30" t="e">
         <f ca="1">F9/F10</f>
-        <v>3.919006354708261</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="30">
+        <v>16</v>
+      </c>
+      <c r="B21" s="30" t="e">
         <f ca="1">F11/F6</f>
-        <v>0.31055914608057289</v>
+        <v>#N/A</v>
       </c>
       <c r="C21" s="25"/>
     </row>
@@ -4138,26 +5909,26 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B23" s="14"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="30">
+        <v>18</v>
+      </c>
+      <c r="B24" s="30" t="e">
         <f ca="1">F8</f>
-        <v>19.79</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="30">
+        <v>13</v>
+      </c>
+      <c r="B25" s="30" t="e">
         <f ca="1">AVERAGE(B8:F8)</f>
-        <v>15.768000000000001</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -4166,41 +5937,42 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="14" t="s">
         <v>23</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="32">
+        <v>19</v>
+      </c>
+      <c r="B28" s="32" t="e">
         <f ca="1">[1]!QFS(INPUT!$B$1, "pe", F3)</f>
-        <v>26.2</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B29" s="27">
-        <v>19.489999999999998</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" s="33">
+        <v>21</v>
+      </c>
+      <c r="B30" s="33" t="e">
         <f ca="1">(B29-B28)/B28</f>
-        <v>-0.25610687022900769</v>
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4209,7 +5981,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -4219,155 +5991,155 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21">
-      <c r="A1" s="106" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
+      <c r="A1" s="118" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="C2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="E2" s="11" t="s">
         <v>28</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="42" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="47">
+        <v>1</v>
+      </c>
+      <c r="B3" s="47" t="e">
         <f ca="1">RATE(1,,-INPUT!E4,INPUT!F4)</f>
-        <v>0.23421586757475973</v>
-      </c>
-      <c r="C3" s="47">
+        <v>#N/A</v>
+      </c>
+      <c r="C3" s="47" t="e">
         <f ca="1">RATE(2,,-INPUT!D4,INPUT!F4)</f>
-        <v>0.23110947474870097</v>
-      </c>
-      <c r="D3" s="47">
+        <v>#N/A</v>
+      </c>
+      <c r="D3" s="47" t="e">
         <f ca="1">RATE(3,,-INPUT!C4,INPUT!F4)</f>
-        <v>0.22193925428985023</v>
-      </c>
-      <c r="E3" s="47">
+        <v>#N/A</v>
+      </c>
+      <c r="E3" s="47" t="e">
         <f ca="1">RATE(4,,-INPUT!B4,INPUT!F4)</f>
-        <v>0.19991083246218541</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="47">
+        <v>2</v>
+      </c>
+      <c r="B4" s="47" t="e">
         <f ca="1">RATE(1,,-INPUT!E5,INPUT!F5)</f>
-        <v>1.427777777777778</v>
-      </c>
-      <c r="C4" s="47">
+        <v>#N/A</v>
+      </c>
+      <c r="C4" s="47" t="e">
         <f ca="1">RATE(2,,-INPUT!D5,INPUT!F5)</f>
-        <v>0.25264531582293448</v>
-      </c>
-      <c r="D4" s="47">
+        <v>#N/A</v>
+      </c>
+      <c r="D4" s="47" t="e">
         <f ca="1">RATE(3,,-INPUT!C5,INPUT!F5)</f>
-        <v>0.24144775025901291</v>
-      </c>
-      <c r="E4" s="47">
+        <v>#N/A</v>
+      </c>
+      <c r="E4" s="47" t="e">
         <f ca="1">RATE(4,,-INPUT!B5,INPUT!F5)</f>
-        <v>0.20729050855011433</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="47">
+        <v>3</v>
+      </c>
+      <c r="B5" s="47" t="e">
         <f ca="1">RATE(1,,-INPUT!E6,INPUT!F6)</f>
-        <v>0.16475849497055775</v>
-      </c>
-      <c r="C5" s="47">
+        <v>#N/A</v>
+      </c>
+      <c r="C5" s="47" t="e">
         <f ca="1">RATE(2,,-INPUT!D6,INPUT!F6)</f>
-        <v>0.13029571332072334</v>
-      </c>
-      <c r="D5" s="47">
+        <v>#N/A</v>
+      </c>
+      <c r="D5" s="47" t="e">
         <f ca="1">RATE(3,,-INPUT!C6,INPUT!F6)</f>
-        <v>0.1386177942897116</v>
-      </c>
-      <c r="E5" s="47">
+        <v>#N/A</v>
+      </c>
+      <c r="E5" s="47" t="e">
         <f ca="1">RATE(4,,-INPUT!B6,INPUT!F6)</f>
-        <v>0.14357796061274317</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="47">
+        <v>4</v>
+      </c>
+      <c r="B6" s="47" t="e">
         <f ca="1">RATE(1,,-INPUT!E7,INPUT!F7)</f>
-        <v>-4.4822127801382922E-2</v>
-      </c>
-      <c r="C6" s="47">
+        <v>#N/A</v>
+      </c>
+      <c r="C6" s="47" t="e">
         <f ca="1">RATE(2,,-INPUT!D7,INPUT!F7)</f>
-        <v>-6.2046099239995232E-2</v>
-      </c>
-      <c r="D6" s="47">
+        <v>#N/A</v>
+      </c>
+      <c r="D6" s="47" t="e">
         <f ca="1">RATE(3,,-INPUT!C7,INPUT!F7)</f>
-        <v>0.11242077175800112</v>
-      </c>
-      <c r="E6" s="47">
+        <v>#N/A</v>
+      </c>
+      <c r="E6" s="47" t="e">
         <f ca="1">RATE(4,,-INPUT!B7,INPUT!F7)</f>
-        <v>0.17413810344383429</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="46" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="47">
+        <v>5</v>
+      </c>
+      <c r="B7" s="47" t="e">
         <f ca="1">RATE(1,,-INPUT!E8,INPUT!F8)</f>
-        <v>1.1557734204793022</v>
-      </c>
-      <c r="C7" s="47">
+        <v>#N/A</v>
+      </c>
+      <c r="C7" s="47" t="e">
         <f ca="1">RATE(2,,-INPUT!D8,INPUT!F8)</f>
-        <v>0.10186679296902529</v>
-      </c>
-      <c r="D7" s="47">
+        <v>#N/A</v>
+      </c>
+      <c r="D7" s="47" t="e">
         <f ca="1">RATE(3,,-INPUT!C8,INPUT!F8)</f>
-        <v>6.5284737673440077E-2</v>
-      </c>
-      <c r="E7" s="47">
+        <v>#N/A</v>
+      </c>
+      <c r="E7" s="47" t="e">
         <f ca="1">RATE(4,,-INPUT!B8,INPUT!F8)</f>
-        <v>3.5688936024080485E-2</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="48">
+        <v>35</v>
+      </c>
+      <c r="B8" s="48" t="e">
         <f ca="1">AVERAGE(B3:B6)</f>
-        <v>0.44548250313042814</v>
-      </c>
-      <c r="C8" s="48">
+        <v>#N/A</v>
+      </c>
+      <c r="C8" s="48" t="e">
         <f t="shared" ref="C8:E8" ca="1" si="0">AVERAGE(C3:C6)</f>
-        <v>0.13800110116309089</v>
-      </c>
-      <c r="D8" s="48">
+        <v>#N/A</v>
+      </c>
+      <c r="D8" s="48" t="e">
         <f t="shared" ca="1" si="0"/>
-        <v>0.17860639264914399</v>
-      </c>
-      <c r="E8" s="48">
+        <v>#N/A</v>
+      </c>
+      <c r="E8" s="48" t="e">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18122935126721931</v>
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>
@@ -4384,7 +6156,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="B8" sqref="B8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -4400,7 +6172,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="8">
         <v>2018</v>
@@ -4422,23 +6194,23 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="42" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="47">
+        <v>1</v>
+      </c>
+      <c r="B3" s="47" t="e">
         <f ca="1">(INPUT!F4 - INPUT!E4) / INPUT!E4</f>
-        <v>0.23421586757475982</v>
-      </c>
-      <c r="C3" s="47">
+        <v>#N/A</v>
+      </c>
+      <c r="C3" s="47" t="e">
         <f ca="1">(INPUT!E4 - INPUT!D4) / INPUT!D4</f>
-        <v>0.22801090038993266</v>
-      </c>
-      <c r="D3" s="47">
+        <v>#N/A</v>
+      </c>
+      <c r="D3" s="47" t="e">
         <f ca="1">(INPUT!D4 - INPUT!C4) / INPUT!C4</f>
-        <v>0.20380322447292271</v>
-      </c>
-      <c r="E3" s="47">
+        <v>#N/A</v>
+      </c>
+      <c r="E3" s="47" t="e">
         <f ca="1">(INPUT!C4 - INPUT!B4) / INPUT!B4</f>
-        <v>0.13617975485219921</v>
+        <v>#N/A</v>
       </c>
       <c r="G3" s="51"/>
       <c r="H3" s="52"/>
@@ -4448,23 +6220,23 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="47">
+        <v>2</v>
+      </c>
+      <c r="B4" s="47" t="e">
         <f ca="1">(INPUT!F5 - INPUT!E5) / INPUT!E5</f>
-        <v>1.427777777777778</v>
-      </c>
-      <c r="C4" s="47">
+        <v>#N/A</v>
+      </c>
+      <c r="C4" s="47" t="e">
         <f ca="1">(INPUT!E5 - INPUT!D5) / INPUT!D5</f>
-        <v>-0.35368043087971279</v>
-      </c>
-      <c r="D4" s="47">
+        <v>#N/A</v>
+      </c>
+      <c r="D4" s="47" t="e">
         <f ca="1">(INPUT!D5 - INPUT!C5) / INPUT!C5</f>
-        <v>0.21935201401050794</v>
-      </c>
-      <c r="E4" s="47">
+        <v>#N/A</v>
+      </c>
+      <c r="E4" s="47" t="e">
         <f ca="1">(INPUT!C5 - INPUT!B5) / INPUT!B5</f>
-        <v>0.11035488575595526</v>
+        <v>#N/A</v>
       </c>
       <c r="G4" s="53"/>
       <c r="H4" s="52"/>
@@ -4474,23 +6246,23 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="47">
+        <v>3</v>
+      </c>
+      <c r="B5" s="47" t="e">
         <f ca="1">(INPUT!F6 - INPUT!E6) / INPUT!E6</f>
-        <v>0.16475849497055775</v>
-      </c>
-      <c r="C5" s="47">
+        <v>#N/A</v>
+      </c>
+      <c r="C5" s="47" t="e">
         <f ca="1">(INPUT!E6 - INPUT!D6) / INPUT!D6</f>
-        <v>9.685261371155672E-2</v>
-      </c>
-      <c r="D5" s="47">
+        <v>#N/A</v>
+      </c>
+      <c r="D5" s="47" t="e">
         <f ca="1">(INPUT!D6 - INPUT!C6) / INPUT!C6</f>
-        <v>0.15544622748917569</v>
-      </c>
-      <c r="E5" s="47">
+        <v>#N/A</v>
+      </c>
+      <c r="E5" s="47" t="e">
         <f ca="1">(INPUT!C6 - INPUT!B6) / INPUT!B6</f>
-        <v>0.15858848449836319</v>
+        <v>#N/A</v>
       </c>
       <c r="G5" s="54"/>
       <c r="H5" s="52"/>
@@ -4500,23 +6272,23 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="47">
+        <v>4</v>
+      </c>
+      <c r="B6" s="47" t="e">
         <f ca="1">(INPUT!F7 - INPUT!E7) / INPUT!E7</f>
-        <v>-4.4822127801382991E-2</v>
-      </c>
-      <c r="C6" s="47">
+        <v>#N/A</v>
+      </c>
+      <c r="C6" s="47" t="e">
         <f ca="1">(INPUT!E7 - INPUT!D7) / INPUT!D7</f>
-        <v>-7.8959484346224684E-2</v>
-      </c>
-      <c r="D6" s="47">
+        <v>#N/A</v>
+      </c>
+      <c r="D6" s="47" t="e">
         <f ca="1">(INPUT!D7 - INPUT!C7) / INPUT!C7</f>
-        <v>0.56474755358107698</v>
-      </c>
-      <c r="E6" s="47">
+        <v>#N/A</v>
+      </c>
+      <c r="E6" s="47" t="e">
         <f ca="1">(INPUT!C7 - INPUT!B7) / INPUT!B7</f>
-        <v>0.38060505594695399</v>
+        <v>#N/A</v>
       </c>
       <c r="G6" s="55"/>
       <c r="H6" s="52"/>
@@ -4526,23 +6298,23 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="46" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="47">
-        <f ca="1">(INPUT!F8 - INPUT!E8) / INPUT!E8</f>
-        <v>1.1557734204793024</v>
-      </c>
-      <c r="C7" s="47">
-        <f ca="1">(INPUT!E8 - INPUT!D8) / INPUT!D8</f>
-        <v>-0.43680981595092017</v>
-      </c>
-      <c r="D7" s="47">
-        <f ca="1">(INPUT!D8 - INPUT!C8) / INPUT!C8</f>
-        <v>-4.276114844227262E-3</v>
-      </c>
-      <c r="E7" s="47">
-        <f ca="1">(INPUT!C8 - INPUT!B8) / INPUT!B8</f>
-        <v>-4.8255813953488276E-2</v>
+        <v>5</v>
+      </c>
+      <c r="B7" s="123" t="e">
+        <f ca="1">INPUT!F8/100</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C7" s="123" t="e">
+        <f ca="1">INPUT!E8/100</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D7" s="123" t="e">
+        <f ca="1">INPUT!D8/100</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E7" s="123" t="e">
+        <f ca="1">INPUT!C8/100</f>
+        <v>#N/A</v>
       </c>
       <c r="G7" s="56"/>
       <c r="H7" s="52"/>
@@ -4552,23 +6324,23 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="57">
+        <v>35</v>
+      </c>
+      <c r="B8" s="57" t="e">
         <f ca="1">AVERAGE(B3:B6)</f>
-        <v>0.4454825031304282</v>
-      </c>
-      <c r="C8" s="57">
-        <f ca="1">AVERAGE(C3:C6)</f>
-        <v>-2.6944100281112025E-2</v>
-      </c>
-      <c r="D8" s="57">
-        <f ca="1">AVERAGE(D3:D6)</f>
-        <v>0.28583725488842082</v>
-      </c>
-      <c r="E8" s="57">
-        <f ca="1">AVERAGE(E3:E6)</f>
-        <v>0.19643204526336791</v>
+        <v>#N/A</v>
+      </c>
+      <c r="C8" s="57" t="e">
+        <f t="shared" ref="C8:E8" ca="1" si="0">AVERAGE(C3:C6)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D8" s="57" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E8" s="57" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#N/A</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="5"/>
@@ -4587,7 +6359,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
@@ -4596,215 +6368,220 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="107" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
+      <c r="A1" s="119" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="119"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="64"/>
-      <c r="B2" s="60" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="60" t="s">
+      <c r="A2" s="62"/>
+      <c r="B2" s="120" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="120" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="120"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="60"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="79" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="66">
-        <v>23.25</v>
-      </c>
-      <c r="C3" s="66">
-        <v>28.465</v>
-      </c>
-      <c r="D3" s="66">
-        <v>33.68</v>
-      </c>
-      <c r="E3" s="66">
-        <v>49.575000000000003</v>
-      </c>
-      <c r="F3" s="66">
-        <v>65.47</v>
+      <c r="B3" s="64" t="e">
+        <f ca="1">B11</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C3" s="64" t="e">
+        <f t="shared" ref="C3:F3" ca="1" si="0">C11</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D3" s="64" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E3" s="64" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F3" s="64" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#N/A</v>
       </c>
       <c r="G3" s="58"/>
       <c r="H3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" s="108">
+        <v>40</v>
+      </c>
+      <c r="I3" s="103" t="e">
         <f ca="1">[1]!QFS(INPUT!$B$1, "eps_diluted", "TTM")</f>
-        <v>39.869999999999997</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="82">
+      <c r="A4" s="79" t="e">
         <f ca="1">A12</f>
-        <v>0.14431249079843397</v>
-      </c>
-      <c r="B4" s="87">
+        <v>#N/A</v>
+      </c>
+      <c r="B4" s="84" t="e">
         <f ca="1">RATE($I$4,,-$I$5,B12)</f>
-        <v>0.12108352279945897</v>
-      </c>
-      <c r="C4" s="83">
-        <f t="shared" ref="C4:F4" ca="1" si="0">RATE($I$4,,-$I$5,C12)</f>
-        <v>0.16461447574353208</v>
-      </c>
-      <c r="D4" s="87">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.2024685363428245</v>
-      </c>
-      <c r="E4" s="83">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.27890320816453368</v>
-      </c>
-      <c r="F4" s="87">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.34050434780410654</v>
+        <v>#N/A</v>
+      </c>
+      <c r="C4" s="80" t="e">
+        <f t="shared" ref="C4:F4" ca="1" si="1">RATE($I$4,,-$I$5,C12)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D4" s="84" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E4" s="80" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F4" s="84" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A</v>
       </c>
       <c r="G4" s="58"/>
       <c r="H4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4" s="108">
+        <v>41</v>
+      </c>
+      <c r="I4" s="103">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="86">
-        <f t="shared" ref="A5:A8" ca="1" si="1">A13</f>
-        <v>0.13029571332072334</v>
-      </c>
-      <c r="B5" s="88">
-        <f t="shared" ref="B5:F5" ca="1" si="2">RATE($I$4,,-$I$5,B13)</f>
-        <v>0.10735127885115096</v>
-      </c>
-      <c r="C5" s="81">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.15034901758894914</v>
-      </c>
-      <c r="D5" s="88">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.18773940069727646</v>
-      </c>
-      <c r="E5" s="81">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.26323781795568368</v>
-      </c>
-      <c r="F5" s="88">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.324084400191615</v>
+      <c r="A5" s="83" t="e">
+        <f t="shared" ref="A5:A8" ca="1" si="2">A13</f>
+        <v>#N/A</v>
+      </c>
+      <c r="B5" s="85" t="e">
+        <f t="shared" ref="B5:F5" ca="1" si="3">RATE($I$4,,-$I$5,B13)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C5" s="78" t="e">
+        <f t="shared" ca="1" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D5" s="85" t="e">
+        <f t="shared" ca="1" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E5" s="78" t="e">
+        <f t="shared" ca="1" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F5" s="85" t="e">
+        <f t="shared" ca="1" si="3"/>
+        <v>#N/A</v>
       </c>
       <c r="G5" s="58"/>
       <c r="H5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" s="109">
+        <v>42</v>
+      </c>
+      <c r="I5" s="104" t="e">
         <f ca="1">[1]!QFS(INPUT!$B$1, "price")</f>
-        <v>1044.6400000000001</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="82">
-        <f t="shared" ca="1" si="1"/>
-        <v>9.0614675633609656E-2</v>
-      </c>
-      <c r="B6" s="87">
-        <f t="shared" ref="B6:F6" ca="1" si="3">RATE($I$4,,-$I$5,B14)</f>
-        <v>6.847574627050243E-2</v>
-      </c>
-      <c r="C6" s="83">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.10996397305388776</v>
-      </c>
-      <c r="D6" s="87">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.14604170038212672</v>
-      </c>
-      <c r="E6" s="83">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.21888961167061613</v>
-      </c>
-      <c r="F6" s="87">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.27760006660905312</v>
+      <c r="A6" s="79" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="B6" s="84" t="e">
+        <f t="shared" ref="B6:F6" ca="1" si="4">RATE($I$4,,-$I$5,B14)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C6" s="80" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D6" s="84" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E6" s="80" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F6" s="84" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#N/A</v>
       </c>
       <c r="G6" s="58"/>
       <c r="H6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" s="109">
+        <v>20</v>
+      </c>
+      <c r="I6" s="104">
         <f>INPUT!B29</f>
-        <v>19.489999999999998</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="86">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.18122935126721931</v>
-      </c>
-      <c r="B7" s="88">
-        <f t="shared" ref="B7:F7" ca="1" si="4">RATE($I$4,,-$I$5,B15)</f>
-        <v>0.15725098956558417</v>
-      </c>
-      <c r="C7" s="81">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.20218630201239468</v>
-      </c>
-      <c r="D7" s="88">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.24126157891727879</v>
-      </c>
-      <c r="E7" s="81">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.32016212272550326</v>
-      </c>
-      <c r="F7" s="88">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.38375058723908179</v>
+      <c r="A7" s="83" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="B7" s="85" t="e">
+        <f t="shared" ref="B7:F7" ca="1" si="5">RATE($I$4,,-$I$5,B15)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C7" s="78" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D7" s="85" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E7" s="78" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F7" s="85" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#N/A</v>
       </c>
       <c r="G7" s="58"/>
       <c r="H7" s="58"/>
       <c r="I7" s="58"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="84">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.22653668908402413</v>
-      </c>
-      <c r="B8" s="80">
-        <f t="shared" ref="B8:F8" ca="1" si="5">RATE($I$4,,-$I$5,B16)</f>
-        <v>0.20163861121329005</v>
-      </c>
-      <c r="C8" s="85">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.24829746649106088</v>
-      </c>
-      <c r="D8" s="80">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.28887151818517887</v>
-      </c>
-      <c r="E8" s="85">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.37079837825292988</v>
-      </c>
-      <c r="F8" s="80">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.43682584755404391</v>
+      <c r="A8" s="81" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="B8" s="77" t="e">
+        <f t="shared" ref="B8:F8" ca="1" si="6">RATE($I$4,,-$I$5,B16)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C8" s="82" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D8" s="77" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E8" s="82" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F8" s="77" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#N/A</v>
       </c>
       <c r="G8" s="58"/>
       <c r="H8" s="58"/>
@@ -4823,314 +6600,314 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="58"/>
-      <c r="B10" s="62" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
+      <c r="B10" s="121" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="121"/>
+      <c r="D10" s="121"/>
+      <c r="E10" s="121"/>
+      <c r="F10" s="121"/>
       <c r="G10" s="58"/>
       <c r="H10" s="58"/>
       <c r="I10" s="58"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="75" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="67">
+      <c r="A11" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="64" t="e">
         <f ca="1">INPUT!$B$15</f>
-        <v>23.647600000000001</v>
-      </c>
-      <c r="C11" s="67">
+        <v>#N/A</v>
+      </c>
+      <c r="C11" s="64" t="e">
         <f ca="1">(B11+D11)/2</f>
-        <v>28.609360000000002</v>
-      </c>
-      <c r="D11" s="67">
+        <v>#N/A</v>
+      </c>
+      <c r="D11" s="64" t="e">
         <f ca="1">INPUT!$B$17</f>
-        <v>33.571120000000001</v>
-      </c>
-      <c r="E11" s="67">
+        <v>#N/A</v>
+      </c>
+      <c r="E11" s="64" t="e">
         <f ca="1">(D11+F11)/2</f>
-        <v>45.686260000000004</v>
-      </c>
-      <c r="F11" s="76">
+        <v>#N/A</v>
+      </c>
+      <c r="F11" s="73" t="e">
         <f ca="1">INPUT!$B$16</f>
-        <v>57.801400000000001</v>
+        <v>#N/A</v>
       </c>
       <c r="G11" s="58"/>
       <c r="H11" s="58"/>
       <c r="I11" s="58"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="69">
+      <c r="A12" s="66" t="e">
         <f ca="1">AVERAGE(GROWTH!B5:E5)</f>
-        <v>0.14431249079843397</v>
-      </c>
-      <c r="B12" s="77">
+        <v>#N/A</v>
+      </c>
+      <c r="B12" s="74" t="e">
         <f ca="1">(B$11*$I$3*(1+$A12)^$I$4)</f>
-        <v>1849.9351270796874</v>
-      </c>
-      <c r="C12" s="77">
-        <f t="shared" ref="C12:F16" ca="1" si="6">(C$11*$I$3*(1+$A12)^$I$4)</f>
-        <v>2238.0901244637312</v>
-      </c>
-      <c r="D12" s="77">
-        <f t="shared" ca="1" si="6"/>
-        <v>2626.2451218477745</v>
-      </c>
-      <c r="E12" s="77">
-        <f t="shared" ca="1" si="6"/>
-        <v>3574.0040088167784</v>
-      </c>
-      <c r="F12" s="70">
-        <f t="shared" ca="1" si="6"/>
-        <v>4521.7628957857814</v>
-      </c>
-      <c r="G12" s="97" t="s">
-        <v>46</v>
+        <v>#N/A</v>
+      </c>
+      <c r="C12" s="74" t="e">
+        <f t="shared" ref="C12:F16" ca="1" si="7">(C$11*$I$3*(1+$A12)^$I$4)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D12" s="74" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E12" s="74" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F12" s="67" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#N/A</v>
+      </c>
+      <c r="G12" s="94" t="s">
+        <v>45</v>
       </c>
       <c r="H12" s="58"/>
       <c r="I12" s="58"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="73">
+      <c r="A13" s="70" t="e">
         <f ca="1">MIN(GROWTH!B5:E5)</f>
-        <v>0.13029571332072334</v>
-      </c>
-      <c r="B13" s="78">
-        <f t="shared" ref="B13:B16" ca="1" si="7">(B$11*$I$3*(1+$A13)^$I$4)</f>
-        <v>1739.3769436654341</v>
-      </c>
-      <c r="C13" s="78">
-        <f t="shared" ca="1" si="6"/>
-        <v>2104.3345268451822</v>
-      </c>
-      <c r="D13" s="78">
-        <f t="shared" ca="1" si="6"/>
-        <v>2469.2921100249296</v>
-      </c>
-      <c r="E13" s="78">
-        <f t="shared" ca="1" si="6"/>
-        <v>3360.4098211363685</v>
-      </c>
-      <c r="F13" s="74">
-        <f t="shared" ca="1" si="6"/>
-        <v>4251.5275322478064</v>
-      </c>
-      <c r="G13" s="98" t="s">
-        <v>47</v>
+        <v>#N/A</v>
+      </c>
+      <c r="B13" s="75" t="e">
+        <f t="shared" ref="B13:B16" ca="1" si="8">(B$11*$I$3*(1+$A13)^$I$4)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C13" s="75" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D13" s="75" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E13" s="75" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F13" s="71" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#N/A</v>
+      </c>
+      <c r="G13" s="95" t="s">
+        <v>46</v>
       </c>
       <c r="H13" s="58"/>
       <c r="I13" s="58"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="69">
+      <c r="A14" s="66" t="e">
         <f ca="1">AVERAGE(GROWTH!E3:E6)/2</f>
-        <v>9.0614675633609656E-2</v>
-      </c>
-      <c r="B14" s="77">
+        <v>#N/A</v>
+      </c>
+      <c r="B14" s="74" t="e">
+        <f t="shared" ca="1" si="8"/>
+        <v>#N/A</v>
+      </c>
+      <c r="C14" s="74" t="e">
         <f t="shared" ca="1" si="7"/>
-        <v>1454.7554512640249</v>
-      </c>
-      <c r="C14" s="77">
-        <f t="shared" ca="1" si="6"/>
-        <v>1759.9935053525494</v>
-      </c>
-      <c r="D14" s="77">
-        <f t="shared" ca="1" si="6"/>
-        <v>2065.2315594410734</v>
-      </c>
-      <c r="E14" s="77">
-        <f t="shared" ca="1" si="6"/>
-        <v>2810.531968693042</v>
-      </c>
-      <c r="F14" s="70">
-        <f t="shared" ca="1" si="6"/>
-        <v>3555.8323779450093</v>
-      </c>
-      <c r="G14" s="99" t="s">
-        <v>49</v>
+        <v>#N/A</v>
+      </c>
+      <c r="D14" s="74" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E14" s="74" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F14" s="67" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#N/A</v>
+      </c>
+      <c r="G14" s="96" t="s">
+        <v>48</v>
       </c>
       <c r="H14" s="58"/>
       <c r="I14" s="58"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="73">
+      <c r="A15" s="70" t="e">
         <f ca="1">AVERAGE(GROWTH!E3:E6)</f>
-        <v>0.18122935126721931</v>
-      </c>
-      <c r="B15" s="78">
+        <v>#N/A</v>
+      </c>
+      <c r="B15" s="75" t="e">
+        <f t="shared" ca="1" si="8"/>
+        <v>#N/A</v>
+      </c>
+      <c r="C15" s="75" t="e">
         <f t="shared" ca="1" si="7"/>
-        <v>2168.2255379922553</v>
-      </c>
-      <c r="C15" s="78">
-        <f t="shared" ca="1" si="6"/>
-        <v>2623.1645062337875</v>
-      </c>
-      <c r="D15" s="78">
-        <f t="shared" ca="1" si="6"/>
-        <v>3078.1034744753192</v>
-      </c>
-      <c r="E15" s="78">
-        <f t="shared" ca="1" si="6"/>
-        <v>4188.9289258679137</v>
-      </c>
-      <c r="F15" s="74">
-        <f t="shared" ca="1" si="6"/>
-        <v>5299.7543772605059</v>
-      </c>
-      <c r="G15" s="99" t="s">
-        <v>48</v>
+        <v>#N/A</v>
+      </c>
+      <c r="D15" s="75" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E15" s="75" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F15" s="71" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#N/A</v>
+      </c>
+      <c r="G15" s="96" t="s">
+        <v>47</v>
       </c>
       <c r="H15" s="58"/>
       <c r="I15" s="58"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="71">
+      <c r="A16" s="68" t="e">
         <f ca="1">AVERAGE(GROWTH!E3:E6)*1.25</f>
-        <v>0.22653668908402413</v>
-      </c>
-      <c r="B16" s="68">
+        <v>#N/A</v>
+      </c>
+      <c r="B16" s="65" t="e">
+        <f t="shared" ca="1" si="8"/>
+        <v>#N/A</v>
+      </c>
+      <c r="C16" s="65" t="e">
         <f t="shared" ca="1" si="7"/>
-        <v>2617.194655249581</v>
-      </c>
-      <c r="C16" s="68">
-        <f t="shared" ca="1" si="6"/>
-        <v>3166.3367141744261</v>
-      </c>
-      <c r="D16" s="68">
-        <f t="shared" ca="1" si="6"/>
-        <v>3715.4787730992707</v>
-      </c>
-      <c r="E16" s="68">
-        <f t="shared" ca="1" si="6"/>
-        <v>5056.3201124149064</v>
-      </c>
-      <c r="F16" s="72">
-        <f t="shared" ca="1" si="6"/>
-        <v>6397.1614517305406</v>
-      </c>
-      <c r="G16" s="98" t="s">
-        <v>50</v>
+        <v>#N/A</v>
+      </c>
+      <c r="D16" s="65" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E16" s="65" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F16" s="69" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#N/A</v>
+      </c>
+      <c r="G16" s="95" t="s">
+        <v>49</v>
       </c>
       <c r="H16" s="58"/>
       <c r="I16" s="58"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="107" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="107"/>
-      <c r="C18" s="107"/>
-      <c r="D18" s="107"/>
-      <c r="E18" s="107"/>
-      <c r="F18" s="107"/>
-      <c r="G18" s="107"/>
-      <c r="H18" s="107"/>
-      <c r="I18" s="107"/>
+      <c r="A18" s="119" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="119"/>
+      <c r="C18" s="119"/>
+      <c r="D18" s="119"/>
+      <c r="E18" s="119"/>
+      <c r="F18" s="119"/>
+      <c r="G18" s="119"/>
+      <c r="H18" s="119"/>
+      <c r="I18" s="119"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="75" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="89">
+      <c r="A19" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="86">
         <f>I6</f>
-        <v>19.489999999999998</v>
-      </c>
-      <c r="C19" s="105"/>
-      <c r="D19" s="93" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="102"/>
+      <c r="D19" s="90" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="88"/>
+      <c r="F19" s="88"/>
+      <c r="G19" s="88"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="66" t="e">
+        <f ca="1">A12</f>
+        <v>#N/A</v>
+      </c>
+      <c r="B20" s="87" t="e">
+        <f ca="1">(B$19*$I$3*(1+$A20)^$I$4)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C20" s="99" t="e">
+        <f ca="1">RATE($I$4,,-$I$5,B20)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D20" s="92" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="89"/>
+      <c r="F20" s="89"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="70" t="e">
+        <f t="shared" ref="A21:A24" ca="1" si="9">A13</f>
+        <v>#N/A</v>
+      </c>
+      <c r="B21" s="97" t="e">
+        <f t="shared" ref="B21:B24" ca="1" si="10">(B$19*$I$3*(1+$A21)^$I$4)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C21" s="100" t="e">
+        <f t="shared" ref="C21:C24" ca="1" si="11">RATE($I$4,,-$I$5,B21)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D21" s="93" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="66" t="e">
+        <f t="shared" ca="1" si="9"/>
+        <v>#N/A</v>
+      </c>
+      <c r="B22" s="87" t="e">
+        <f t="shared" ca="1" si="10"/>
+        <v>#N/A</v>
+      </c>
+      <c r="C22" s="99" t="e">
+        <f t="shared" ca="1" si="11"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D22" s="91" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="70" t="e">
+        <f t="shared" ca="1" si="9"/>
+        <v>#N/A</v>
+      </c>
+      <c r="B23" s="97" t="e">
+        <f t="shared" ca="1" si="10"/>
+        <v>#N/A</v>
+      </c>
+      <c r="C23" s="101" t="e">
+        <f t="shared" ca="1" si="11"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D23" s="91" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="91"/>
-      <c r="F19" s="91"/>
-      <c r="G19" s="91"/>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="69">
-        <f ca="1">A12</f>
-        <v>0.14431249079843397</v>
-      </c>
-      <c r="B20" s="90">
-        <f ca="1">(B$19*$I$3*(1+$A20)^$I$4)</f>
-        <v>1524.6890012848282</v>
-      </c>
-      <c r="C20" s="102">
-        <f ca="1">RATE($I$4,,-$I$5,B20)</f>
-        <v>7.855655651370759E-2</v>
-      </c>
-      <c r="D20" s="95" t="s">
-        <v>51</v>
-      </c>
-      <c r="E20" s="92"/>
-      <c r="F20" s="92"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="73">
-        <f t="shared" ref="A21:A24" ca="1" si="8">A13</f>
-        <v>0.13029571332072334</v>
-      </c>
-      <c r="B21" s="100">
-        <f t="shared" ref="B21:B24" ca="1" si="9">(B$19*$I$3*(1+$A21)^$I$4)</f>
-        <v>1433.5685918249339</v>
-      </c>
-      <c r="C21" s="103">
-        <f t="shared" ref="C21:C24" ca="1" si="10">RATE($I$4,,-$I$5,B21)</f>
-        <v>6.534522886028897E-2</v>
-      </c>
-      <c r="D21" s="96" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="69">
-        <f t="shared" ca="1" si="8"/>
-        <v>9.0614675633609656E-2</v>
-      </c>
-      <c r="B22" s="90">
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="68" t="e">
         <f t="shared" ca="1" si="9"/>
-        <v>1198.9877934816152</v>
-      </c>
-      <c r="C22" s="102">
+        <v>#N/A</v>
+      </c>
+      <c r="B24" s="98" t="e">
         <f t="shared" ca="1" si="10"/>
-        <v>2.794439324186335E-2</v>
-      </c>
-      <c r="D22" s="94" t="s">
+        <v>#N/A</v>
+      </c>
+      <c r="C24" s="100" t="e">
+        <f t="shared" ca="1" si="11"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D24" s="93" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="73">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.18122935126721931</v>
-      </c>
-      <c r="B23" s="100">
-        <f t="shared" ca="1" si="9"/>
-        <v>1787.0192212093004</v>
-      </c>
-      <c r="C23" s="104">
-        <f t="shared" ca="1" si="10"/>
-        <v>0.11335205356591267</v>
-      </c>
-      <c r="D23" s="94" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="71">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.22653668908402413</v>
-      </c>
-      <c r="B24" s="101">
-        <f t="shared" ca="1" si="9"/>
-        <v>2157.0528861624152</v>
-      </c>
-      <c r="C24" s="103">
-        <f t="shared" ca="1" si="10"/>
-        <v>0.15605588372862519</v>
-      </c>
-      <c r="D24" s="96" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -5147,10 +6924,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6BB3CFD-76EF-9945-B6B4-5335762D9010}">
-  <dimension ref="A3:K15"/>
+  <dimension ref="A3:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -5166,238 +6943,264 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:11">
-      <c r="A3" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="60"/>
-      <c r="D3" s="60" t="s">
+      <c r="A3" s="120" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="120"/>
+      <c r="D3" s="120" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="120"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="120" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="60"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="60" t="s">
+      <c r="H3" s="120"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="120" t="s">
         <v>58</v>
       </c>
-      <c r="H3" s="60"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="60" t="s">
-        <v>59</v>
-      </c>
-      <c r="K3" s="60"/>
+      <c r="K3" s="120"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="63">
+        <v>40</v>
+      </c>
+      <c r="B4" s="61" t="e">
         <f ca="1">[1]!QFS(INPUT!$B$1, "eps_diluted", "TTM")</f>
-        <v>39.869999999999997</v>
+        <v>#N/A</v>
       </c>
       <c r="C4" s="58"/>
       <c r="D4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="110">
+        <v>59</v>
+      </c>
+      <c r="E4" s="105" t="e">
         <f ca="1">AVERAGE(GROWTH!E3:E6)</f>
-        <v>0.18122935126721931</v>
+        <v>#N/A</v>
       </c>
       <c r="F4" s="58"/>
       <c r="G4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H4" s="120">
+        <v>59</v>
+      </c>
+      <c r="H4" s="115">
         <v>0.15</v>
       </c>
       <c r="I4" s="58"/>
       <c r="J4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="K4" s="112">
+        <v>60</v>
+      </c>
+      <c r="K4" s="107" t="e">
         <f ca="1">INPUT!F7</f>
-        <v>22930</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="63">
+        <v>41</v>
+      </c>
+      <c r="B5" s="61">
         <v>5</v>
       </c>
       <c r="C5" s="58"/>
-      <c r="D5" s="113" t="s">
-        <v>62</v>
-      </c>
-      <c r="E5" s="61">
+      <c r="D5" s="108" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="60" t="e">
         <f ca="1">(B4*INPUT!B17*(1+E4)^B5)/(1+B8)^B5</f>
-        <v>1530.3614363499621</v>
+        <v>#N/A</v>
       </c>
       <c r="F5" s="58"/>
-      <c r="G5" s="113" t="s">
-        <v>62</v>
-      </c>
-      <c r="H5" s="61">
+      <c r="G5" s="108" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="60" t="e">
         <f ca="1">(B4*INPUT!B17*(1+H4)^B5)/(1+B8)^B5</f>
-        <v>1338.4805543999998</v>
+        <v>#N/A</v>
       </c>
       <c r="I5" s="58"/>
       <c r="J5" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="K5" s="114">
+        <v>62</v>
+      </c>
+      <c r="K5" s="109" t="e">
         <f ca="1">[1]!QFS(INPUT!$B$1, "mkt_cap")</f>
-        <v>732166</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="61" t="e">
+        <f ca="1">[1]!QFS(INPUT!$B$1, "price")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C6" s="58"/>
+      <c r="D6" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="63">
-        <f ca="1">[1]!QFS(INPUT!$B$1, "price")</f>
-        <v>1044.6400000000001</v>
-      </c>
-      <c r="C6" s="58"/>
-      <c r="D6" s="115" t="s">
-        <v>65</v>
-      </c>
-      <c r="E6" s="61">
+      <c r="E6" s="60" t="e">
         <f ca="1">E5*(1-B7)</f>
-        <v>1147.7710772624716</v>
+        <v>#N/A</v>
       </c>
       <c r="F6" s="58"/>
-      <c r="G6" s="115" t="s">
-        <v>65</v>
-      </c>
-      <c r="H6" s="61">
+      <c r="G6" s="110" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="60" t="e">
         <f ca="1">H5*(1-B7)</f>
-        <v>1003.8604157999998</v>
+        <v>#N/A</v>
       </c>
       <c r="I6" s="58"/>
       <c r="J6" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K6" s="114">
+        <v>59</v>
+      </c>
+      <c r="K6" s="109">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="106">
+        <v>0.25</v>
+      </c>
+      <c r="C7" s="58"/>
+      <c r="D7" s="111" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="111">
-        <v>0.25</v>
-      </c>
-      <c r="C7" s="58"/>
-      <c r="D7" s="116" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" s="61">
+      <c r="E7" s="60" t="e">
         <f ca="1">E5</f>
-        <v>1530.3614363499621</v>
+        <v>#N/A</v>
       </c>
       <c r="F7" s="58"/>
-      <c r="G7" s="116" t="s">
-        <v>67</v>
-      </c>
-      <c r="H7" s="61">
+      <c r="G7" s="111" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="60" t="e">
         <f ca="1">H5</f>
-        <v>1338.4805543999998</v>
+        <v>#N/A</v>
       </c>
       <c r="I7" s="58"/>
       <c r="J7" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="K7" s="117">
+        <v>58</v>
+      </c>
+      <c r="K7" s="112" t="e">
         <f ca="1">LN(1+K6*(K5/K4+1))/LN(1+K6)-1</f>
-        <v>1.237790036482258</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="111">
+        <v>67</v>
+      </c>
+      <c r="B8" s="106">
         <v>0.15</v>
       </c>
       <c r="C8" s="58"/>
       <c r="D8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E8" s="118" t="str">
+        <v>68</v>
+      </c>
+      <c r="E8" s="113" t="e">
         <f ca="1">_xlfn.IFS(B6&lt;E6,"BUY",B6&gt;E7,"SELL",B6&lt;E7,"HOLD")</f>
-        <v>BUY</v>
+        <v>#N/A</v>
       </c>
       <c r="F8" s="58"/>
       <c r="G8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H8" s="119" t="str">
+        <v>68</v>
+      </c>
+      <c r="H8" s="114" t="e">
         <f ca="1">_xlfn.IFS(B6&lt;H6,"BUY",B6&gt;H7,"SELL",B6&lt;H7,"HOLD")</f>
-        <v>HOLD</v>
+        <v>#N/A</v>
       </c>
       <c r="I8" s="58"/>
       <c r="J8" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="K8" s="118" t="str">
+        <v>69</v>
+      </c>
+      <c r="K8" s="113" t="e">
         <f ca="1">_xlfn.IFS(K7&gt;8,"NO",K7&lt;8,"YES", K7=8, "YES")</f>
-        <v>YES</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="D10" s="60" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="60"/>
+      <c r="D10" s="120" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="120"/>
     </row>
     <row r="11" spans="1:11">
       <c r="D11" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E11" s="110">
+        <v>70</v>
+      </c>
+      <c r="E11" s="105" t="e">
         <f ca="1">AVERAGE(GROWTH!B5:E5)</f>
-        <v>0.14431249079843397</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="D12" s="113" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="61">
+      <c r="D12" s="108" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="60" t="e">
         <f ca="1">(B4*INPUT!B17*(1+E11)^B5)/(1+B8)^B5</f>
-        <v>1305.7079757733361</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="D13" s="115" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" s="61">
+      <c r="D13" s="110" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="60" t="e">
         <f ca="1">E12*(1-B7)</f>
-        <v>979.28098183000202</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="D14" s="116" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" s="61">
+      <c r="D14" s="111" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="60" t="e">
         <f ca="1">E12</f>
-        <v>1305.7079757733361</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="D15" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" s="118" t="str">
+        <v>68</v>
+      </c>
+      <c r="E15" s="113" t="e">
         <f ca="1">_xlfn.IFS(B6&lt;E13,"BUY",B6&gt;E14,"SELL",B6&lt;E14,"HOLD")</f>
-        <v>HOLD</v>
-      </c>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="122" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="122"/>
+      <c r="D18" s="122"/>
+      <c r="E18" s="122"/>
+      <c r="F18" s="122"/>
+      <c r="G18" s="122"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="B19" s="117" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="116"/>
+      <c r="D19" s="116"/>
+      <c r="E19" s="116"/>
+      <c r="F19" s="116"/>
+      <c r="G19" s="116"/>
+      <c r="H19" s="116"/>
+      <c r="I19" s="116"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="B18:G18"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="G3:H3"/>

</xml_diff>